<commit_message>
Latest changes to support AML and cervical projects
</commit_message>
<xml_diff>
--- a/doc/drop/drop_all_tables.xlsx
+++ b/doc/drop/drop_all_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjg994/Documents/omop-abstractor/doc/drop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3FE7E9-38A2-404E-B17D-8741EF779B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8009D083-C411-5A4D-8492-2296C1BD28D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="760" windowWidth="28040" windowHeight="16420" xr2:uid="{FD8A4D80-FF6B-7046-BDFE-BE595F8073DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>cohort_definition</t>
   </si>
@@ -42,9 +42,6 @@
     <t>cohort</t>
   </si>
   <si>
-    <t>cohort_attribute</t>
-  </si>
-  <si>
     <t>concept_ancestor</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>ar_internal_metadata</t>
   </si>
   <si>
-    <t>attribute_definition</t>
-  </si>
-  <si>
     <t>cdm_source</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>abstractor_object_value_variants</t>
   </si>
   <si>
-    <t>abstractor_relation_types</t>
-  </si>
-  <si>
     <t>abstractor_rule_abstractor_subjects</t>
   </si>
   <si>
@@ -255,30 +246,15 @@
     <t>abstractor_subjects</t>
   </si>
   <si>
-    <t>articles</t>
-  </si>
-  <si>
-    <t>encounter_notes</t>
-  </si>
-  <si>
-    <t>imaging_exams</t>
-  </si>
-  <si>
     <t>login_audits</t>
   </si>
   <si>
-    <t>moomins</t>
-  </si>
-  <si>
     <t>note_stable_identifier</t>
   </si>
   <si>
     <t>note_stable_identifier_full</t>
   </si>
   <si>
-    <t>pathology_cases</t>
-  </si>
-  <si>
     <t>pii_address</t>
   </si>
   <si>
@@ -297,9 +273,6 @@
     <t>procedure_occurrence_stable_identifier</t>
   </si>
   <si>
-    <t>radiation_therapy_prescriptions</t>
-  </si>
-  <si>
     <t>site_categories</t>
   </si>
   <si>
@@ -312,15 +285,6 @@
     <t>sql_audits</t>
   </si>
   <si>
-    <t>surgeries</t>
-  </si>
-  <si>
-    <t>surgical_procedure_reports</t>
-  </si>
-  <si>
-    <t>surgical_procedures</t>
-  </si>
-  <si>
     <t>users</t>
   </si>
   <si>
@@ -360,9 +324,6 @@
     <t>nlp_comparisons</t>
   </si>
   <si>
-    <t>abstractions</t>
-  </si>
-  <si>
     <t>batch_pathology_report_sections</t>
   </si>
   <si>
@@ -391,6 +352,30 @@
   </si>
   <si>
     <t>sessions</t>
+  </si>
+  <si>
+    <t>aml_pathology_cases</t>
+  </si>
+  <si>
+    <t>patients</t>
+  </si>
+  <si>
+    <t>primary_cns_pathology_cases</t>
+  </si>
+  <si>
+    <t>ohdsi_nlp_proposal_pathology_cases</t>
+  </si>
+  <si>
+    <t>prostate_surgery_pathology_cases</t>
+  </si>
+  <si>
+    <t>breast_pathology_cases</t>
+  </si>
+  <si>
+    <t>episode</t>
+  </si>
+  <si>
+    <t>episode_event</t>
   </si>
 </sst>
 </file>
@@ -742,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A31C0B-F15F-A245-8B8C-E2CB9577C12E}">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B119" sqref="B1:B119"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,47 +741,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" t="str">
         <f t="shared" ref="B1:B32" si="0">CONCATENATE("DROP TABLE ",A1, " CASCADE;")</f>
-        <v>DROP TABLE abstractor_abstraction_schema_relations CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_schema_predicate_variants CASCADE;</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractions CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_schema_object_values CASCADE;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_group_members CASCADE;</v>
+        <v>DROP TABLE abstractor_rule_types CASCADE;</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_groups CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_schemas CASCADE;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_object_values CASCADE;</v>
+        <v>DROP TABLE drug_exposure CASCADE;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -805,237 +790,237 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_schema_object_values CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_schema_relations CASCADE;</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_schema_predicate_variants CASCADE;</v>
+        <v>DROP TABLE abstractor_subject_relations CASCADE;</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_source_types CASCADE;</v>
+        <v>DROP TABLE abstractor_subjects CASCADE;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_schemas CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_group_members CASCADE;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_source_sections CASCADE;</v>
+        <v>DROP TABLE schema_migrations CASCADE;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstraction_sources CASCADE;</v>
+        <v>DROP TABLE abstractor_suggestion_object_values CASCADE;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_abstractions CASCADE;</v>
+        <v>DROP TABLE abstractor_subject_group_members CASCADE;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_indirect_sources CASCADE;</v>
+        <v>DROP TABLE abstractor_abstractions CASCADE;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_namespace_events CASCADE;</v>
+        <v>DROP TABLE abstractor_suggestions CASCADE;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_namespace_sections CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_groups CASCADE;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_namespaces CASCADE;</v>
+        <v>DROP TABLE abstractor_subject_groups CASCADE;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_object_value_variants CASCADE;</v>
+        <v>DROP TABLE procedure_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_object_types CASCADE;</v>
+        <v>DROP TABLE aml_pathology_cases CASCADE;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_object_values CASCADE;</v>
+        <v>DROP TABLE abstractor_section_types CASCADE;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_relation_types CASCADE;</v>
+        <v>DROP TABLE abstractor_section_name_variants CASCADE;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_rule_abstractor_subjects CASCADE;</v>
+        <v>DROP TABLE abstractor_sections CASCADE;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_rule_types CASCADE;</v>
+        <v>DROP TABLE abstractor_object_values CASCADE;</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_rules CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_object_values CASCADE;</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_section_mention_types CASCADE;</v>
+        <v>DROP TABLE abstractor_rules CASCADE;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_section_name_variants CASCADE;</v>
+        <v>DROP TABLE abstractor_rule_abstractor_subjects CASCADE;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_section_types CASCADE;</v>
+        <v>DROP TABLE cdm_source CASCADE;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_sections CASCADE;</v>
+        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_subject_group_members CASCADE;</v>
+        <v>DROP TABLE care_site CASCADE;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_subject_groups CASCADE;</v>
+        <v>DROP TABLE person CASCADE;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_subject_relations CASCADE;</v>
+        <v>DROP TABLE visit_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>DROP TABLE abstractor_subjects CASCADE;</v>
+        <v>DROP TABLE visit_detail CASCADE;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -1044,65 +1029,65 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" ref="B33:B64" si="1">CONCATENATE("DROP TABLE ",A33, " CASCADE;")</f>
-        <v>DROP TABLE abstractor_suggestion_object_values CASCADE;</v>
+        <v>DROP TABLE versions CASCADE;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE abstractor_suggestion_sources CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_sources CASCADE;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE abstractor_suggestions CASCADE;</v>
+        <v>DROP TABLE concept CASCADE;</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE api_logs CASCADE;</v>
+        <v>DROP TABLE cohort CASCADE;</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE ar_internal_metadata CASCADE;</v>
+        <v>DROP TABLE cohort_definition CASCADE;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE articles CASCADE;</v>
+        <v>DROP TABLE cost CASCADE;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE attribute_definition CASCADE;</v>
+        <v>DROP TABLE fact_relationship CASCADE;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1111,718 +1096,673 @@
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE cdm_source CASCADE;</v>
+        <v>DROP TABLE location CASCADE;</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE batch_nu_chers_pathology_report_sections CASCADE;</v>
+        <v>DROP TABLE sites CASCADE;</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE batch_pathology_report_sections CASCADE;</v>
+        <v>DROP TABLE note_nlp CASCADE;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE case_numbers CASCADE;</v>
+        <v>DROP TABLE device_exposure CASCADE;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE cohort_definition CASCADE;</v>
+        <v>DROP TABLE metadata CASCADE;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE compare_breast_cancer_abstractions CASCADE;</v>
+        <v>DROP TABLE vocabulary CASCADE;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE compare_cancer_abstractions CASCADE;</v>
+        <v>DROP TABLE source_to_concept_map CASCADE;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE compare_cancer_diagnosis_abstractions CASCADE;</v>
+        <v>DROP TABLE drug_strength CASCADE;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE compare_pspore_surgeries CASCADE;</v>
+        <v>DROP TABLE domain CASCADE;</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE cohort_attribute CASCADE;</v>
+        <v>DROP TABLE concept_class CASCADE;</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE concept_ancestor CASCADE;</v>
+        <v>DROP TABLE concept_relationship CASCADE;</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE concept_class CASCADE;</v>
+        <v>DROP TABLE relationship CASCADE;</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE domain CASCADE;</v>
+        <v>DROP TABLE site_categories_sites CASCADE;</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE concept_synonym CASCADE;</v>
+        <v>DROP TABLE site_categories CASCADE;</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE fact_relationship CASCADE;</v>
+        <v>DROP TABLE measurement CASCADE;</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE concept_relationship CASCADE;</v>
+        <v>DROP TABLE pii_email CASCADE;</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE drug_strength CASCADE;</v>
+        <v>DROP TABLE pii_mrn CASCADE;</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE condition_era CASCADE;</v>
+        <v>DROP TABLE pii_name CASCADE;</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE death CASCADE;</v>
+        <v>DROP TABLE pii_phone_number CASCADE;</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE condition_occurrence CASCADE;</v>
+        <v>DROP TABLE concept_ancestor CASCADE;</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE encounter_notes CASCADE;</v>
+        <v>DROP TABLE users CASCADE;</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE icdo3_categories CASCADE;</v>
+        <v>DROP TABLE login_audits CASCADE;</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE concept CASCADE;</v>
+        <v>DROP TABLE patients CASCADE;</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE icdo3_categorizations CASCADE;</v>
+        <v>DROP TABLE note CASCADE;</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="1"/>
-        <v>DROP TABLE icdo3_histologies CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_source_sections CASCADE;</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" ref="B65:B96" si="2">CONCATENATE("DROP TABLE ",A65, " CASCADE;")</f>
-        <v>DROP TABLE icdo3_histology_synonyms CASCADE;</v>
+        <v>DROP TABLE abstractor_section_mention_types CASCADE;</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE icdo3_site_synonyms CASCADE;</v>
+        <v>DROP TABLE nlp_comparisons CASCADE;</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE imaging_exams CASCADE;</v>
+        <v>DROP TABLE icdo3_histologies CASCADE;</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE icdo3_sites CASCADE;</v>
+        <v>DROP TABLE icdo3_histology_synonyms CASCADE;</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE location CASCADE;</v>
+        <v>DROP TABLE note_stable_identifier CASCADE;</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE login_audits CASCADE;</v>
+        <v>DROP TABLE abstractor_object_types CASCADE;</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE moomins CASCADE;</v>
+        <v>DROP TABLE icdo3_sites CASCADE;</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE metadata CASCADE;</v>
+        <v>DROP TABLE icdo3_site_synonyms CASCADE;</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE nlp_comparison_suggestions CASCADE;</v>
+        <v>DROP TABLE icdo3_categories CASCADE;</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE measurement CASCADE;</v>
+        <v>DROP TABLE icdo3_categorizations CASCADE;</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE nlp_comparisons CASCADE;</v>
+        <v>DROP TABLE batch_pathology_report_sections CASCADE;</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE note_nlp CASCADE;</v>
+        <v>DROP TABLE case_numbers CASCADE;</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pathology_cases CASCADE;</v>
+        <v>DROP TABLE compare_pspore_surgeries CASCADE;</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE note_stable_identifier CASCADE;</v>
+        <v>DROP TABLE batch_pathology_case_surgeries CASCADE;</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pathology_accession_numbers CASCADE;</v>
+        <v>DROP TABLE sessions CASCADE;</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pii_mrn CASCADE;</v>
+        <v>DROP TABLE primary_cns_pathology_cases CASCADE;</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B81" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pii_name CASCADE;</v>
+        <v>DROP TABLE drug_era CASCADE;</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B82" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pii_phone_number CASCADE;</v>
+        <v>DROP TABLE ohdsi_nlp_proposal_pathology_cases CASCADE;</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE note_stable_identifier_full CASCADE;</v>
+        <v>DROP TABLE condition_occurrence CASCADE;</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE note CASCADE;</v>
+        <v>DROP TABLE abstractor_object_value_variants CASCADE;</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE person CASCADE;</v>
+        <v>DROP TABLE prostate_surgery_pathology_cases CASCADE;</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE observation CASCADE;</v>
+        <v>DROP TABLE observation_period CASCADE;</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pii_address CASCADE;</v>
+        <v>DROP TABLE abstractor_suggestion_sources CASCADE;</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE pii_email CASCADE;</v>
+        <v>DROP TABLE death CASCADE;</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE procedure_occurrence_stable_identifier CASCADE;</v>
+        <v>DROP TABLE abstractor_abstraction_source_types CASCADE;</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE specimen CASCADE;</v>
+        <v>DROP TABLE abstractor_indirect_sources CASCADE;</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE radiation_therapy_prescriptions CASCADE;</v>
+        <v>DROP TABLE pii_address CASCADE;</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE schema_migrations CASCADE;</v>
+        <v>DROP TABLE concept_synonym CASCADE;</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE site_categories CASCADE;</v>
+        <v>DROP TABLE abstractor_namespaces CASCADE;</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE site_categories_sites CASCADE;</v>
+        <v>DROP TABLE api_logs CASCADE;</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE sites CASCADE;</v>
+        <v>DROP TABLE abstractor_namespace_events CASCADE;</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="2"/>
-        <v>DROP TABLE sql_audits CASCADE;</v>
+        <v>DROP TABLE breast_pathology_cases CASCADE;</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" ref="B97:B119" si="3">CONCATENATE("DROP TABLE ",A97, " CASCADE;")</f>
-        <v>DROP TABLE surgeries CASCADE;</v>
+        <v>DROP TABLE provider CASCADE;</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE surgical_procedure_reports CASCADE;</v>
+        <v>DROP TABLE dose_era CASCADE;</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE relationship CASCADE;</v>
+        <v>DROP TABLE procedure_occurrence_stable_identifier CASCADE;</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE surgical_procedures CASCADE;</v>
+        <v>DROP TABLE sql_audits CASCADE;</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE provider CASCADE;</v>
+        <v>DROP TABLE abstractor_namespace_sections CASCADE;</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE source_to_concept_map CASCADE;</v>
+        <v>DROP TABLE nlp_comparison_suggestions CASCADE;</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE users CASCADE;</v>
+        <v>DROP TABLE condition_era CASCADE;</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE versions CASCADE;</v>
+        <v>DROP TABLE episode CASCADE;</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE vocabulary CASCADE;</v>
+        <v>DROP TABLE pathology_accession_numbers CASCADE;</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE sessions CASCADE;</v>
+        <v>DROP TABLE batch_nu_chers_pathology_report_sections CASCADE;</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE visit_occurrence CASCADE;</v>
+        <v>DROP TABLE compare_cancer_diagnosis_abstractions CASCADE;</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE batch_pathology_case_surgeries CASCADE;</v>
+        <v>DROP TABLE compare_cancer_abstractions CASCADE;</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE cohort CASCADE;</v>
+        <v>DROP TABLE compare_breast_cancer_abstractions CASCADE;</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE care_site CASCADE;</v>
+        <v>DROP TABLE episode_event CASCADE;</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE procedure_occurrence CASCADE;</v>
+        <v>DROP TABLE observation CASCADE;</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE drug_era CASCADE;</v>
+        <v>DROP TABLE payer_plan_period CASCADE;</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE device_exposure CASCADE;</v>
+        <v>DROP TABLE specimen CASCADE;</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="3"/>
-        <v>DROP TABLE drug_exposure CASCADE;</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>12</v>
-      </c>
-      <c r="B115" t="str">
-        <f t="shared" si="3"/>
-        <v>DROP TABLE dose_era CASCADE;</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>18</v>
-      </c>
-      <c r="B116" t="str">
-        <f t="shared" si="3"/>
-        <v>DROP TABLE observation_period CASCADE;</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>29</v>
-      </c>
-      <c r="B117" t="str">
-        <f t="shared" si="3"/>
-        <v>DROP TABLE payer_plan_period CASCADE;</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" t="str">
-        <f t="shared" si="3"/>
-        <v>DROP TABLE cost CASCADE;</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" t="str">
-        <f t="shared" si="3"/>
-        <v>DROP TABLE visit_detail CASCADE;</v>
+        <v>DROP TABLE note_stable_identifier_full CASCADE;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>